<commit_message>
remain only one choice of gas (fossil fuel)
</commit_message>
<xml_diff>
--- a/cea_energy_hub_optimizer/data/example_techDefinition_daily.xlsx
+++ b/cea_energy_hub_optimizer/data/example_techDefinition_daily.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangy\Documents\GitHub\energy_hub_optimizer_calliope\cea_energy_hub_optimizer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A220AFDB-E277-4CD9-8215-6FEBD66B48D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78D3644-3969-454E-96FD-3FBB869126B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="620" windowWidth="31430" windowHeight="18170" xr2:uid="{3D0A62A3-FD81-47EE-AB31-50A82C57680E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{3D0A62A3-FD81-47EE-AB31-50A82C57680E}"/>
   </bookViews>
   <sheets>
     <sheet name="supply" sheetId="5" r:id="rId1"/>
@@ -118,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{29079865-22BD-4294-8AAF-CA614A3F9A35}">
+    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{29079865-22BD-4294-8AAF-CA614A3F9A35}">
       <text>
         <r>
           <rPr>
@@ -143,7 +143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{33A05C13-4314-4914-82EE-E11B048CC5C7}">
+    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{33A05C13-4314-4914-82EE-E11B048CC5C7}">
       <text>
         <r>
           <rPr>
@@ -167,7 +167,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{B664C2FD-AA61-4A19-91B5-C6D3502ACED2}">
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{B664C2FD-AA61-4A19-91B5-C6D3502ACED2}">
       <text>
         <r>
           <rPr>
@@ -192,7 +192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{F979F4B1-5E70-4C02-B7AD-A61C2F5CB7BC}">
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{F979F4B1-5E70-4C02-B7AD-A61C2F5CB7BC}">
       <text>
         <r>
           <rPr>
@@ -2097,7 +2097,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="132">
   <si>
     <t>monetary</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2111,14 +2111,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>gas_individuell</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>gas_erneuerbar</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PV_small</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2212,10 +2204,6 @@
   </si>
   <si>
     <t>#094926</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#fabf8f</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -3084,10 +3072,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2603C43B-861B-457A-A24B-3EBFF53534AD}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -3105,19 +3093,19 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
       <c r="I1" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -3130,38 +3118,38 @@
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -3169,13 +3157,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E4">
         <v>0.2505</v>
@@ -3198,13 +3186,13 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E5">
         <v>0.13250000000000001</v>
@@ -3224,26 +3212,25 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="E6">
-        <v>0.14299999999999999</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="F6">
         <v>0.05</v>
       </c>
       <c r="G6">
-        <f>AVERAGE(G5,G7)</f>
-        <v>0.17699999999999999</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -3254,25 +3241,25 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="E7">
-        <v>0.17799999999999999</v>
+        <v>0.1</v>
       </c>
       <c r="F7">
         <v>0.05</v>
       </c>
       <c r="G7">
-        <v>0.124</v>
+        <v>0.32400000000000001</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -3286,85 +3273,27 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E8">
-        <v>0.10199999999999999</v>
+        <v>0.122</v>
       </c>
       <c r="F8">
         <v>0.05</v>
       </c>
       <c r="G8">
-        <v>2.8000000000000001E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>98</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9">
-        <v>0.1</v>
-      </c>
-      <c r="F9">
-        <v>0.05</v>
-      </c>
-      <c r="G9">
-        <v>0.32400000000000001</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" t="s">
-        <v>98</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10">
-        <v>0.122</v>
-      </c>
-      <c r="F10">
-        <v>0.05</v>
-      </c>
-      <c r="G10">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
         <v>1</v>
       </c>
     </row>
@@ -3414,13 +3343,13 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -3428,7 +3357,7 @@
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
@@ -3450,7 +3379,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
       <c r="I2" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
@@ -3464,72 +3393,72 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E4">
         <v>3000</v>
@@ -3550,19 +3479,19 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="L4" t="b">
         <v>1</v>
       </c>
       <c r="M4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="N4">
         <v>5</v>
       </c>
       <c r="O4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="P4">
         <v>1</v>
@@ -3576,16 +3505,16 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E5">
         <v>1444</v>
@@ -3606,19 +3535,19 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="L5" t="b">
         <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="N5">
         <v>5</v>
       </c>
       <c r="O5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="P5">
         <v>10</v>
@@ -3632,16 +3561,16 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E6">
         <v>1284</v>
@@ -3662,19 +3591,19 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="L6" t="b">
         <v>1</v>
       </c>
       <c r="M6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="N6">
         <v>5</v>
       </c>
       <c r="O6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="P6">
         <v>100</v>
@@ -3688,16 +3617,16 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E7">
         <v>1576</v>
@@ -3715,13 +3644,13 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="L7" t="b">
         <v>1</v>
       </c>
       <c r="M7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="N7">
         <v>1.2969999999999999</v>
@@ -3735,16 +3664,16 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E8">
         <v>2047</v>
@@ -3762,13 +3691,13 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="L8" t="b">
         <v>1</v>
       </c>
       <c r="M8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="N8">
         <v>1.41</v>
@@ -3823,14 +3752,14 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
@@ -3838,7 +3767,7 @@
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
@@ -3857,7 +3786,7 @@
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
@@ -3867,66 +3796,66 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F4">
         <v>371.80000000000013</v>
@@ -3961,19 +3890,19 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F5">
         <v>180.88</v>
@@ -4008,19 +3937,19 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F6">
         <v>117.4</v>
@@ -4055,19 +3984,19 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F7">
         <v>72.010000000000005</v>
@@ -4102,19 +4031,19 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F8">
         <v>1814.5</v>
@@ -4149,19 +4078,19 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C9" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F9">
         <v>2544.9</v>
@@ -4196,19 +4125,19 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F10">
         <v>1814.5</v>
@@ -4243,19 +4172,19 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F11">
         <v>2544.9</v>
@@ -4290,19 +4219,19 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F12">
         <v>1814.5</v>
@@ -4337,19 +4266,19 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F13">
         <v>2544.9</v>
@@ -4384,19 +4313,19 @@
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F14">
         <v>300</v>
@@ -4431,19 +4360,19 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F15">
         <v>880</v>
@@ -4478,19 +4407,19 @@
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F16">
         <v>486.7</v>
@@ -4525,19 +4454,19 @@
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F17">
         <v>176.7</v>
@@ -4572,19 +4501,19 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F18">
         <v>414.99999999999989</v>
@@ -4619,19 +4548,19 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F19">
         <v>189.4</v>
@@ -4666,19 +4595,19 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F20">
         <v>155.30000000000001</v>
@@ -4713,19 +4642,19 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
         <v>48</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" t="s">
-        <v>100</v>
-      </c>
-      <c r="D21" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" t="s">
-        <v>51</v>
       </c>
       <c r="F21">
         <v>278.00000000000006</v>
@@ -4760,19 +4689,19 @@
     </row>
     <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C22" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F22">
         <v>211.7</v>
@@ -4807,16 +4736,16 @@
     </row>
     <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C23" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E23" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G23">
         <v>0.05</v>
@@ -4833,16 +4762,16 @@
     </row>
     <row r="24" spans="1:15">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C24" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E24" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G24">
         <v>0.05</v>
@@ -4908,7 +4837,7 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -4919,7 +4848,7 @@
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
       <c r="J1" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
@@ -4928,7 +4857,7 @@
       <c r="O1" s="8"/>
       <c r="P1" s="8"/>
       <c r="Q1" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R1" s="8"/>
       <c r="S1" s="8"/>
@@ -4956,7 +4885,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -4970,72 +4899,72 @@
     </row>
     <row r="3" spans="1:24">
       <c r="A3" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F3" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="L3" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="I3" s="8" t="s">
+      <c r="M3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="R3" s="9" t="s">
         <v>105</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>108</v>
       </c>
       <c r="S3" s="9"/>
       <c r="T3" s="9"/>
       <c r="U3" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="V3" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="W3" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="X3" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:24">
@@ -5057,11 +4986,11 @@
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
       <c r="R4" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="S4" s="9"/>
       <c r="T4" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="U4" s="9"/>
       <c r="V4" s="8"/>
@@ -5087,13 +5016,13 @@
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="U5" s="9"/>
       <c r="V5" s="8"/>
@@ -5102,22 +5031,22 @@
     </row>
     <row r="6" spans="1:24">
       <c r="A6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
         <v>91</v>
       </c>
-      <c r="C6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" t="s">
-        <v>94</v>
-      </c>
       <c r="H6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J6">
         <v>1108.2</v>
@@ -5149,7 +5078,7 @@
         <v>0.64</v>
       </c>
       <c r="U6" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="V6">
         <v>10</v>
@@ -5163,6 +5092,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="Q3:Q5"/>
+    <mergeCell ref="W3:W5"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="U3:U5"/>
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="J1:P1"/>
     <mergeCell ref="D3:D5"/>
@@ -5179,18 +5120,6 @@
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="X3:X5"/>
     <mergeCell ref="A1:I2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="Q3:Q5"/>
-    <mergeCell ref="W3:W5"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="I3:I5"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="U3:U5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5227,20 +5156,20 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
       <c r="J1" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
@@ -5259,7 +5188,7 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -5271,63 +5200,63 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E4">
         <v>367</v>
@@ -5365,16 +5294,16 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E5">
         <v>13</v>
@@ -5409,16 +5338,16 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E6">
         <v>13</v>
@@ -5453,16 +5382,16 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E7">
         <v>13</v>
@@ -5528,13 +5457,13 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -5546,121 +5475,121 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" t="s">
         <v>114</v>
       </c>
-      <c r="B4" t="s">
-        <v>117</v>
-      </c>
       <c r="C4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" t="s">
         <v>118</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
         <v>121</v>
-      </c>
-      <c r="D5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" t="s">
         <v>121</v>
-      </c>
-      <c r="D6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" t="s">
         <v>121</v>
-      </c>
-      <c r="D7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" t="s">
         <v>119</v>
       </c>
-      <c r="C8" t="s">
-        <v>121</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>122</v>
-      </c>
-      <c r="E8" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
global sensitivity for supply technologies running
</commit_message>
<xml_diff>
--- a/cea_energy_hub_optimizer/data/example_techDefinition_daily.xlsx
+++ b/cea_energy_hub_optimizer/data/example_techDefinition_daily.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangy\Documents\GitHub\energy_hub_optimizer_calliope\cea_energy_hub_optimizer\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yiqwang\Documents\GitHub\energy_hub_optimizer_calliope\cea_energy_hub_optimizer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78D3644-3969-454E-96FD-3FBB869126B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611908B2-4B42-444A-837E-9E0813B5DEEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{3D0A62A3-FD81-47EE-AB31-50A82C57680E}"/>
+    <workbookView xWindow="4440" yWindow="4095" windowWidth="38700" windowHeight="15345" activeTab="1" xr2:uid="{3D0A62A3-FD81-47EE-AB31-50A82C57680E}"/>
   </bookViews>
   <sheets>
     <sheet name="supply" sheetId="5" r:id="rId1"/>
@@ -32,8 +32,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -468,7 +466,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{E12426D1-3981-473D-8372-399B69C9CB5F}">
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{E12426D1-3981-473D-8372-399B69C9CB5F}">
       <text>
         <r>
           <rPr>
@@ -496,7 +494,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{F8D9F75B-0547-4549-8288-A925727BEEAA}">
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{F8D9F75B-0547-4549-8288-A925727BEEAA}">
       <text>
         <r>
           <rPr>
@@ -520,7 +518,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N7" authorId="0" shapeId="0" xr:uid="{B542349D-BC24-4C65-A89F-1B47531CAF34}">
+    <comment ref="N8" authorId="0" shapeId="0" xr:uid="{B542349D-BC24-4C65-A89F-1B47531CAF34}">
       <text>
         <r>
           <rPr>
@@ -544,7 +542,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O7" authorId="0" shapeId="0" xr:uid="{DD74A52F-1054-45EF-9073-B14456474A5B}">
+    <comment ref="O8" authorId="0" shapeId="0" xr:uid="{DD74A52F-1054-45EF-9073-B14456474A5B}">
       <text>
         <r>
           <rPr>
@@ -568,7 +566,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R7" authorId="0" shapeId="0" xr:uid="{2DCFA103-1274-4847-83A7-AC3F88F17291}">
+    <comment ref="R8" authorId="0" shapeId="0" xr:uid="{2DCFA103-1274-4847-83A7-AC3F88F17291}">
       <text>
         <r>
           <rPr>
@@ -592,7 +590,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{27610EE9-A3A8-40CA-8A0D-BE26099C4505}">
+    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{27610EE9-A3A8-40CA-8A0D-BE26099C4505}">
       <text>
         <r>
           <rPr>
@@ -616,7 +614,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N8" authorId="0" shapeId="0" xr:uid="{BF918F83-D58B-46AA-AB83-02772C77D60C}">
+    <comment ref="N9" authorId="0" shapeId="0" xr:uid="{BF918F83-D58B-46AA-AB83-02772C77D60C}">
       <text>
         <r>
           <rPr>
@@ -640,7 +638,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R8" authorId="0" shapeId="0" xr:uid="{960AF645-C149-407D-B0B9-2EF4831D05BD}">
+    <comment ref="R9" authorId="0" shapeId="0" xr:uid="{960AF645-C149-407D-B0B9-2EF4831D05BD}">
       <text>
         <r>
           <rPr>
@@ -1657,10 +1655,20 @@
     </comment>
     <comment ref="X6" authorId="1" shapeId="0" xr:uid="{4BB9E1A7-B022-46AE-9E98-BC8F14DC2BFC}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <charset val="134"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     from ChatGPT, need revision</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -2097,7 +2105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="134">
   <si>
     <t>monetary</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2398,217 +2406,221 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>energy_per_area</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCFP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>carrier_in</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>carrier_out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GSHP_60</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GSHP_85</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HEX_85_60</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HEX_60_35</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gas_micro_CHP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>carrier_in_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>carrier_out_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>heat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>parent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>storage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>parent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>supply</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>supply</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>conversion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>storage_loss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>storage_initial</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interest_rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interest_rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>primary_carrier_out</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>primary_carrier_in</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>conversion_plus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>carrier_ratios</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>export</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>resource</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df=supply_SCET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df=supply_SCFP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>demand_electricity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>demand_space_cooling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>demand_hot_water</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#aeff60</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#fac710</t>
+  </si>
+  <si>
+    <t>#12cdd4</t>
+  </si>
+  <si>
+    <t>#ff6728</t>
+  </si>
+  <si>
+    <t>demand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cooling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df=demand_electricity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df=demand_space_heating</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df=demand_space_cooling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df=demand_hot_water</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>storage_cap_max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>demand_space_heating_35</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#fcd510</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#ffa210</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>demand_space_heating_60</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>demand_space_heating_85</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>force_resource</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>purchase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PV_extra_large</t>
+  </si>
+  <si>
+    <t>#c69874</t>
+  </si>
+  <si>
     <t>resource_area_per_energy_cap</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>energy_per_area</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SCFP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SCET</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>carrier_in</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>carrier_out</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GSHP_60</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GSHP_85</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HEX_85_60</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HEX_60_35</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>gas_micro_CHP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>carrier_in_2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>carrier_out_2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>heat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>parent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>storage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>parent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>supply</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>supply</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>conversion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>storage_loss</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>storage_initial</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interest_rate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interest_rate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>primary_carrier_out</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>primary_carrier_in</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>conversion_plus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>carrier_ratios</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>export</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>resource</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>df=supply_PV</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>df=supply_SCET</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>df=supply_SCFP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>demand_electricity</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>demand_space_cooling</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>demand_hot_water</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#aeff60</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#fac710</t>
-  </si>
-  <si>
-    <t>#12cdd4</t>
-  </si>
-  <si>
-    <t>#ff6728</t>
-  </si>
-  <si>
-    <t>demand</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cooling</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>df=demand_electricity</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>df=demand_space_heating</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>df=demand_space_cooling</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>df=demand_hot_water</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>storage_cap_max</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>demand_space_heating_35</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#fcd510</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#ffa210</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>demand_space_heating_60</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>demand_space_heating_85</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>force_resource</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>purchase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>supply_for_pv</t>
   </si>
 </sst>
 </file>
@@ -2619,14 +2631,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2648,26 +2660,26 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -3074,24 +3086,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2603C43B-861B-457A-A24B-3EBFF53534AD}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.9140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.9140625" customWidth="1"/>
+    <col min="4" max="4" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.875" customWidth="1"/>
     <col min="7" max="7" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.4140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="15">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -3108,7 +3120,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" ht="15">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -3123,7 +3135,7 @@
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" ht="15">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -3131,22 +3143,22 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>17</v>
@@ -3160,7 +3172,7 @@
         <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
@@ -3189,7 +3201,7 @@
         <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D5" t="s">
         <v>33</v>
@@ -3218,7 +3230,7 @@
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -3247,7 +3259,7 @@
         <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -3276,7 +3288,7 @@
         <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -3313,35 +3325,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{561E90E2-20B4-48EB-B5A5-7E82D5B88F8D}">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="12.9140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.875" customWidth="1"/>
+    <col min="7" max="7" width="14.875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" customWidth="1"/>
-    <col min="11" max="11" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.1640625" customWidth="1"/>
+    <col min="9" max="9" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.875" customWidth="1"/>
+    <col min="11" max="11" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.125" customWidth="1"/>
     <col min="13" max="13" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.08203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.58203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" ht="15">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -3367,7 +3379,7 @@
       <c r="Q1" s="8"/>
       <c r="R1" s="8"/>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" ht="15">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -3391,7 +3403,7 @@
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" ht="15">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -3399,40 +3411,40 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>77</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>76</v>
@@ -3455,44 +3467,12 @@
         <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
+        <v>133</v>
       </c>
       <c r="E4">
         <v>3000</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" s="7">
-        <v>-0.12720000000000001</v>
-      </c>
-      <c r="H4">
-        <v>0.05</v>
-      </c>
-      <c r="I4">
-        <v>1250</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4" t="s">
-        <v>108</v>
-      </c>
-      <c r="L4" t="b">
-        <v>1</v>
-      </c>
-      <c r="M4" t="s">
-        <v>79</v>
-      </c>
-      <c r="N4">
-        <v>5</v>
-      </c>
-      <c r="O4" t="s">
-        <v>32</v>
-      </c>
+      <c r="G4" s="7"/>
       <c r="P4">
         <v>1</v>
       </c>
@@ -3511,44 +3491,12 @@
         <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D5" t="s">
-        <v>32</v>
+        <v>133</v>
       </c>
       <c r="E5">
-        <v>1444</v>
-      </c>
-      <c r="F5">
-        <v>15555.6</v>
-      </c>
-      <c r="G5" s="7">
-        <v>-0.12720000000000001</v>
-      </c>
-      <c r="H5">
-        <v>0.05</v>
-      </c>
-      <c r="I5">
-        <v>1250</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5" t="s">
-        <v>108</v>
-      </c>
-      <c r="L5" t="b">
-        <v>1</v>
-      </c>
-      <c r="M5" t="s">
-        <v>79</v>
-      </c>
-      <c r="N5">
-        <v>5</v>
-      </c>
-      <c r="O5" t="s">
-        <v>32</v>
-      </c>
+        <v>1600</v>
+      </c>
+      <c r="G5" s="7"/>
       <c r="P5">
         <v>10</v>
       </c>
@@ -3567,49 +3515,17 @@
         <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D6" t="s">
-        <v>32</v>
+        <v>133</v>
       </c>
       <c r="E6">
-        <v>1284</v>
-      </c>
-      <c r="F6">
-        <v>31579</v>
-      </c>
-      <c r="G6" s="7">
-        <v>-0.12720000000000001</v>
-      </c>
-      <c r="H6">
-        <v>0.05</v>
-      </c>
-      <c r="I6">
-        <v>1250</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6" t="s">
-        <v>108</v>
-      </c>
-      <c r="L6" t="b">
-        <v>1</v>
-      </c>
-      <c r="M6" t="s">
-        <v>79</v>
-      </c>
-      <c r="N6">
-        <v>5</v>
-      </c>
-      <c r="O6" t="s">
-        <v>32</v>
-      </c>
+        <v>1300</v>
+      </c>
+      <c r="G6" s="7"/>
       <c r="P6">
         <v>100</v>
       </c>
       <c r="Q6">
-        <v>2000</v>
+        <v>200</v>
       </c>
       <c r="R6">
         <v>27</v>
@@ -3617,66 +3533,43 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>130</v>
+      </c>
+      <c r="B7" t="s">
+        <v>131</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D7" t="s">
-        <v>75</v>
+        <v>133</v>
       </c>
       <c r="E7">
-        <v>1576</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>0.05</v>
-      </c>
-      <c r="I7">
-        <v>290</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7" t="s">
-        <v>110</v>
-      </c>
-      <c r="L7" t="b">
-        <v>1</v>
-      </c>
-      <c r="M7" t="s">
-        <v>79</v>
-      </c>
-      <c r="N7">
-        <v>1.2969999999999999</v>
-      </c>
+        <v>1000</v>
+      </c>
+      <c r="G7" s="7"/>
       <c r="P7">
-        <v>1</v>
+        <v>200</v>
+      </c>
+      <c r="Q7">
+        <v>2000</v>
       </c>
       <c r="R7">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="E8">
-        <v>2047</v>
+        <v>1576</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -3685,27 +3578,74 @@
         <v>0.05</v>
       </c>
       <c r="I8">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L8" t="b">
         <v>1</v>
       </c>
       <c r="M8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N8">
-        <v>1.41</v>
+        <v>1.2969999999999999</v>
       </c>
       <c r="P8">
         <v>1</v>
       </c>
       <c r="R8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9">
+        <v>2047</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0.05</v>
+      </c>
+      <c r="I9">
+        <v>296</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
+        <v>107</v>
+      </c>
+      <c r="L9" t="b">
+        <v>1</v>
+      </c>
+      <c r="M9" t="s">
+        <v>78</v>
+      </c>
+      <c r="N9">
+        <v>1.41</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="R9">
         <v>23</v>
       </c>
     </row>
@@ -3731,26 +3671,26 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.75" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.58203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" customWidth="1"/>
-    <col min="12" max="12" width="10.08203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.875" customWidth="1"/>
+    <col min="12" max="12" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.58203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" ht="15">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -3773,7 +3713,7 @@
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" ht="15">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -3794,7 +3734,7 @@
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" ht="15">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -3802,19 +3742,19 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>13</v>
@@ -3826,7 +3766,7 @@
         <v>14</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>20</v>
@@ -3849,7 +3789,7 @@
         <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -3896,7 +3836,7 @@
         <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -3943,7 +3883,7 @@
         <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -3990,7 +3930,7 @@
         <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -4037,7 +3977,7 @@
         <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D8" t="s">
         <v>32</v>
@@ -4084,7 +4024,7 @@
         <v>58</v>
       </c>
       <c r="C9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D9" t="s">
         <v>32</v>
@@ -4131,7 +4071,7 @@
         <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D10" t="s">
         <v>32</v>
@@ -4172,13 +4112,13 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D11" t="s">
         <v>32</v>
@@ -4225,7 +4165,7 @@
         <v>61</v>
       </c>
       <c r="C12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D12" t="s">
         <v>32</v>
@@ -4266,13 +4206,13 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D13" t="s">
         <v>32</v>
@@ -4319,7 +4259,7 @@
         <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D14" t="s">
         <v>33</v>
@@ -4366,7 +4306,7 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
@@ -4413,7 +4353,7 @@
         <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
@@ -4460,7 +4400,7 @@
         <v>63</v>
       </c>
       <c r="C17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D17" t="s">
         <v>33</v>
@@ -4507,7 +4447,7 @@
         <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D18" t="s">
         <v>10</v>
@@ -4554,7 +4494,7 @@
         <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
@@ -4601,7 +4541,7 @@
         <v>66</v>
       </c>
       <c r="C20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D20" t="s">
         <v>33</v>
@@ -4648,7 +4588,7 @@
         <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D21" t="s">
         <v>10</v>
@@ -4695,7 +4635,7 @@
         <v>68</v>
       </c>
       <c r="C22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
@@ -4736,10 +4676,10 @@
     </row>
     <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D23" t="s">
         <v>48</v>
@@ -4762,10 +4702,10 @@
     </row>
     <row r="24" spans="1:15">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D24" t="s">
         <v>75</v>
@@ -4808,34 +4748,34 @@
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.58203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.58203125" customWidth="1"/>
+    <col min="15" max="15" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.625" customWidth="1"/>
     <col min="17" max="17" width="10.25" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="7.75" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.25" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12.25" customWidth="1"/>
-    <col min="22" max="22" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" ht="15">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -4867,7 +4807,7 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" ht="15">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -4897,7 +4837,7 @@
       <c r="W2" s="8"/>
       <c r="X2" s="8"/>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" ht="15">
       <c r="A3" s="8" t="s">
         <v>24</v>
       </c>
@@ -4905,34 +4845,34 @@
         <v>7</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="H3" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>90</v>
-      </c>
       <c r="I3" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>14</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M3" s="8" t="s">
         <v>13</v>
@@ -4944,13 +4884,13 @@
         <v>14</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q3" s="8" t="s">
         <v>20</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="S3" s="9"/>
       <c r="T3" s="9"/>
@@ -4967,7 +4907,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" ht="15">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -4986,18 +4926,18 @@
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
       <c r="R4" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="S4" s="9"/>
       <c r="T4" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="U4" s="9"/>
       <c r="V4" s="8"/>
       <c r="W4" s="8"/>
       <c r="X4" s="8"/>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" ht="15">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -5029,24 +4969,24 @@
       <c r="W5" s="8"/>
       <c r="X5" s="8"/>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" ht="14.25">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6" t="s">
         <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H6" t="s">
         <v>32</v>
       </c>
       <c r="I6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J6">
         <v>1108.2</v>
@@ -5092,18 +5032,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="Q3:Q5"/>
-    <mergeCell ref="W3:W5"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="I3:I5"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="U3:U5"/>
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="J1:P1"/>
     <mergeCell ref="D3:D5"/>
@@ -5120,6 +5048,18 @@
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="X3:X5"/>
     <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="Q3:Q5"/>
+    <mergeCell ref="W3:W5"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="U3:U5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5135,26 +5075,26 @@
       <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.5" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="16.5" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.4140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.4140625" customWidth="1"/>
-    <col min="10" max="10" width="10.08203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.375" customWidth="1"/>
+    <col min="10" max="10" width="10.125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.08203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.75" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.58203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" ht="15">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -5177,7 +5117,7 @@
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" ht="15">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -5198,7 +5138,7 @@
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" ht="15">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -5206,7 +5146,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
@@ -5218,34 +5158,34 @@
         <v>74</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>72</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>20</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>73</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" ht="27">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -5253,7 +5193,7 @@
         <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
@@ -5292,7 +5232,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" ht="27">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -5300,7 +5240,7 @@
         <v>29</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
         <v>51</v>
@@ -5336,7 +5276,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" ht="27">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -5344,7 +5284,7 @@
         <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D6" t="s">
         <v>75</v>
@@ -5380,7 +5320,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" ht="27">
       <c r="A7" t="s">
         <v>71</v>
       </c>
@@ -5388,7 +5328,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D7" t="s">
         <v>48</v>
@@ -5446,13 +5386,13 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -5473,7 +5413,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" ht="15">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -5481,115 +5421,115 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D5" t="s">
         <v>51</v>
       </c>
       <c r="E5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D6" t="s">
         <v>75</v>
       </c>
       <c r="E6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D7" t="s">
         <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" t="s">
         <v>116</v>
       </c>
-      <c r="C8" t="s">
-        <v>118</v>
-      </c>
       <c r="D8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D9" t="s">
         <v>75</v>
       </c>
       <c r="E9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prepare for sensitivity analysis for conversion technologies (WIP).
Currently, setting=setting_all_grouped.
</commit_message>
<xml_diff>
--- a/cea_energy_hub_optimizer/data/example_techDefinition_daily.xlsx
+++ b/cea_energy_hub_optimizer/data/example_techDefinition_daily.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yiqwang\Documents\GitHub\energy_hub_optimizer_calliope\cea_energy_hub_optimizer\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangy\Documents\GitHub\energy_hub_optimizer_calliope\cea_energy_hub_optimizer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611908B2-4B42-444A-837E-9E0813B5DEEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508D3F99-6B10-4FC8-86A3-1394914DDB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="4095" windowWidth="38700" windowHeight="15345" activeTab="1" xr2:uid="{3D0A62A3-FD81-47EE-AB31-50A82C57680E}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15943" xr2:uid="{3D0A62A3-FD81-47EE-AB31-50A82C57680E}"/>
   </bookViews>
   <sheets>
     <sheet name="supply" sheetId="5" r:id="rId1"/>
@@ -68,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{BF94E0D0-CF1A-4E6A-826E-30BA18B65D8A}">
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{BF94E0D0-CF1A-4E6A-826E-30BA18B65D8A}">
       <text>
         <r>
           <rPr>
@@ -92,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{5F07713E-B53A-4F68-B948-0DE6093B4E37}">
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{5F07713E-B53A-4F68-B948-0DE6093B4E37}">
       <text>
         <r>
           <rPr>
@@ -141,7 +141,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{33A05C13-4314-4914-82EE-E11B048CC5C7}">
+    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{33A05C13-4314-4914-82EE-E11B048CC5C7}">
       <text>
         <r>
           <rPr>
@@ -190,7 +190,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{F979F4B1-5E70-4C02-B7AD-A61C2F5CB7BC}">
+    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{F979F4B1-5E70-4C02-B7AD-A61C2F5CB7BC}">
       <text>
         <r>
           <rPr>
@@ -249,7 +249,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{381592D0-4B82-44EA-8DB3-F97383AB5D21}">
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{381592D0-4B82-44EA-8DB3-F97383AB5D21}">
       <text>
         <r>
           <rPr>
@@ -273,7 +273,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{61312002-E024-4292-93F4-FD63A14A1DFD}">
+    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{61312002-E024-4292-93F4-FD63A14A1DFD}">
       <text>
         <r>
           <rPr>
@@ -298,31 +298,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{A439E244-A83C-403E-BC74-150106BD9060}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yiqiao Wang:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-in case that carrier can be sold back to the grid, specify the name of the carrier</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{F156C5E5-9988-454F-B199-E54895C12234}">
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{F156C5E5-9988-454F-B199-E54895C12234}">
       <text>
         <r>
           <rPr>
@@ -346,7 +322,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{AEFC007F-1ADD-4627-B6DF-D92185D067E3}">
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{AEFC007F-1ADD-4627-B6DF-D92185D067E3}">
       <text>
         <r>
           <rPr>
@@ -370,7 +346,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="0" shapeId="0" xr:uid="{164D751A-85F8-4A50-833D-EAAD0DAA59C2}">
+    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{164D751A-85F8-4A50-833D-EAAD0DAA59C2}">
       <text>
         <r>
           <rPr>
@@ -442,7 +418,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{637B0CCF-82B9-4C6D-A8BB-FCB6633100EF}">
+    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{637B0CCF-82B9-4C6D-A8BB-FCB6633100EF}">
       <text>
         <r>
           <rPr>
@@ -494,7 +470,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{F8D9F75B-0547-4549-8288-A925727BEEAA}">
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{F8D9F75B-0547-4549-8288-A925727BEEAA}">
       <text>
         <r>
           <rPr>
@@ -518,7 +494,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N8" authorId="0" shapeId="0" xr:uid="{B542349D-BC24-4C65-A89F-1B47531CAF34}">
+    <comment ref="K8" authorId="0" shapeId="0" xr:uid="{B542349D-BC24-4C65-A89F-1B47531CAF34}">
       <text>
         <r>
           <rPr>
@@ -542,31 +518,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O8" authorId="0" shapeId="0" xr:uid="{DD74A52F-1054-45EF-9073-B14456474A5B}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yiqiao Wang:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-empty cells will not be translated into yaml files and calliope will use its default value for this. However, it is possible that calliope also doesn't have a default value, during which an error might occur.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="R8" authorId="0" shapeId="0" xr:uid="{2DCFA103-1274-4847-83A7-AC3F88F17291}">
+    <comment ref="N8" authorId="0" shapeId="0" xr:uid="{2DCFA103-1274-4847-83A7-AC3F88F17291}">
       <text>
         <r>
           <rPr>
@@ -590,7 +542,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{27610EE9-A3A8-40CA-8A0D-BE26099C4505}">
+    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{27610EE9-A3A8-40CA-8A0D-BE26099C4505}">
       <text>
         <r>
           <rPr>
@@ -614,7 +566,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N9" authorId="0" shapeId="0" xr:uid="{BF918F83-D58B-46AA-AB83-02772C77D60C}">
+    <comment ref="K9" authorId="0" shapeId="0" xr:uid="{BF918F83-D58B-46AA-AB83-02772C77D60C}">
       <text>
         <r>
           <rPr>
@@ -638,7 +590,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R9" authorId="0" shapeId="0" xr:uid="{960AF645-C149-407D-B0B9-2EF4831D05BD}">
+    <comment ref="N9" authorId="0" shapeId="0" xr:uid="{960AF645-C149-407D-B0B9-2EF4831D05BD}">
       <text>
         <r>
           <rPr>
@@ -697,7 +649,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{BDBEED3E-46FF-4A68-AB32-4FA2E417A8AB}">
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{BDBEED3E-46FF-4A68-AB32-4FA2E417A8AB}">
       <text>
         <r>
           <rPr>
@@ -722,7 +674,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{FAF47280-A22A-4725-83CF-2FFB2495B647}">
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{FAF47280-A22A-4725-83CF-2FFB2495B647}">
       <text>
         <r>
           <rPr>
@@ -746,7 +698,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{34B10223-7A34-446D-BC14-3CEB6051B6A9}">
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{34B10223-7A34-446D-BC14-3CEB6051B6A9}">
       <text>
         <r>
           <rPr>
@@ -770,7 +722,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{F68FE046-B4A1-4E11-A3F9-22AEA125C71A}">
+    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{F68FE046-B4A1-4E11-A3F9-22AEA125C71A}">
       <text>
         <r>
           <rPr>
@@ -794,7 +746,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{2A5008E0-6771-496C-A929-12D90B68E371}">
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{2A5008E0-6771-496C-A929-12D90B68E371}">
       <text>
         <r>
           <rPr>
@@ -818,7 +770,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{2E9194AA-01A3-4783-B5CF-A05FF31A6CD7}">
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{2E9194AA-01A3-4783-B5CF-A05FF31A6CD7}">
       <text>
         <r>
           <rPr>
@@ -866,7 +818,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J4" authorId="0" shapeId="0" xr:uid="{297D4FF6-CDCE-45D9-A6E8-AC5B9C4D197D}">
+    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{297D4FF6-CDCE-45D9-A6E8-AC5B9C4D197D}">
       <text>
         <r>
           <rPr>
@@ -938,7 +890,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{BDFC9954-A248-4855-8C3F-B57A2113B405}">
+    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{BDFC9954-A248-4855-8C3F-B57A2113B405}">
       <text>
         <r>
           <rPr>
@@ -962,7 +914,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L8" authorId="0" shapeId="0" xr:uid="{8D30FF0A-F524-4BAB-A2A9-55CA0982EF14}">
+    <comment ref="J8" authorId="0" shapeId="0" xr:uid="{8D30FF0A-F524-4BAB-A2A9-55CA0982EF14}">
       <text>
         <r>
           <rPr>
@@ -987,7 +939,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O8" authorId="0" shapeId="0" xr:uid="{21E87ED6-F24A-4DA0-A3F6-1520504A752B}">
+    <comment ref="M8" authorId="0" shapeId="0" xr:uid="{21E87ED6-F24A-4DA0-A3F6-1520504A752B}">
       <text>
         <r>
           <rPr>
@@ -1011,7 +963,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L9" authorId="0" shapeId="0" xr:uid="{0E42BBB0-E2D2-4B44-A8FB-B6C155C3EBB8}">
+    <comment ref="J9" authorId="0" shapeId="0" xr:uid="{0E42BBB0-E2D2-4B44-A8FB-B6C155C3EBB8}">
       <text>
         <r>
           <rPr>
@@ -1060,7 +1012,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{641049B0-A4A9-4070-BE17-D18C9F965D2B}">
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{641049B0-A4A9-4070-BE17-D18C9F965D2B}">
       <text>
         <r>
           <rPr>
@@ -1084,7 +1036,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O10" authorId="0" shapeId="0" xr:uid="{F03E95D3-22AC-4F5A-A01A-E49103ED38DC}">
+    <comment ref="M10" authorId="0" shapeId="0" xr:uid="{F03E95D3-22AC-4F5A-A01A-E49103ED38DC}">
       <text>
         <r>
           <rPr>
@@ -1108,7 +1060,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L11" authorId="0" shapeId="0" xr:uid="{C5D0AF4C-BF2F-4C21-9650-2E8E580F6C8C}">
+    <comment ref="J11" authorId="0" shapeId="0" xr:uid="{C5D0AF4C-BF2F-4C21-9650-2E8E580F6C8C}">
       <text>
         <r>
           <rPr>
@@ -1156,7 +1108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I12" authorId="0" shapeId="0" xr:uid="{09CB5F3B-6E04-4BCC-A37A-F3ABBAD7BD61}">
+    <comment ref="H12" authorId="0" shapeId="0" xr:uid="{09CB5F3B-6E04-4BCC-A37A-F3ABBAD7BD61}">
       <text>
         <r>
           <rPr>
@@ -1180,7 +1132,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O12" authorId="0" shapeId="0" xr:uid="{0C0424B8-830D-41AF-9090-E6C9C5134069}">
+    <comment ref="M12" authorId="0" shapeId="0" xr:uid="{0C0424B8-830D-41AF-9090-E6C9C5134069}">
       <text>
         <r>
           <rPr>
@@ -1228,7 +1180,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I14" authorId="0" shapeId="0" xr:uid="{AB00EA6B-EDC9-4CF5-B490-4899A5405AC4}">
+    <comment ref="H14" authorId="0" shapeId="0" xr:uid="{AB00EA6B-EDC9-4CF5-B490-4899A5405AC4}">
       <text>
         <r>
           <rPr>
@@ -1252,7 +1204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J15" authorId="0" shapeId="0" xr:uid="{32220E44-B3A9-4388-B223-558CBD5E3D40}">
+    <comment ref="I15" authorId="0" shapeId="0" xr:uid="{32220E44-B3A9-4388-B223-558CBD5E3D40}">
       <text>
         <r>
           <rPr>
@@ -1276,7 +1228,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I17" authorId="0" shapeId="0" xr:uid="{4A7C72F0-7DE0-4554-AF5C-D1918452E588}">
+    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{4A7C72F0-7DE0-4554-AF5C-D1918452E588}">
       <text>
         <r>
           <rPr>
@@ -1300,7 +1252,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J18" authorId="0" shapeId="0" xr:uid="{8B7A05C7-D040-4169-AD2E-35122D0CCCDF}">
+    <comment ref="I18" authorId="0" shapeId="0" xr:uid="{8B7A05C7-D040-4169-AD2E-35122D0CCCDF}">
       <text>
         <r>
           <rPr>
@@ -1324,7 +1276,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I20" authorId="0" shapeId="0" xr:uid="{CB1A0D7B-E5FD-4735-8255-AA5171D239DF}">
+    <comment ref="H20" authorId="0" shapeId="0" xr:uid="{CB1A0D7B-E5FD-4735-8255-AA5171D239DF}">
       <text>
         <r>
           <rPr>
@@ -1348,7 +1300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J21" authorId="0" shapeId="0" xr:uid="{6FC2FE87-96A6-4E67-8D36-DD5F481FA6F9}">
+    <comment ref="I21" authorId="0" shapeId="0" xr:uid="{6FC2FE87-96A6-4E67-8D36-DD5F481FA6F9}">
       <text>
         <r>
           <rPr>
@@ -1372,7 +1324,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O23" authorId="0" shapeId="0" xr:uid="{AF2745AD-0BD1-40F0-B7C8-39776BC84E0B}">
+    <comment ref="M23" authorId="0" shapeId="0" xr:uid="{AF2745AD-0BD1-40F0-B7C8-39776BC84E0B}">
       <text>
         <r>
           <rPr>
@@ -1655,20 +1607,10 @@
     </comment>
     <comment ref="X6" authorId="1" shapeId="0" xr:uid="{4BB9E1A7-B022-46AE-9E98-BC8F14DC2BFC}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <charset val="134"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     from ChatGPT, need revision</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -1730,7 +1672,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{838C1899-AD71-407A-892C-57CED5C28137}">
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{838C1899-AD71-407A-892C-57CED5C28137}">
       <text>
         <r>
           <rPr>
@@ -1754,7 +1696,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{F0749ECF-8748-463A-AB60-85E38149A943}">
+    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{F0749ECF-8748-463A-AB60-85E38149A943}">
       <text>
         <r>
           <rPr>
@@ -1778,7 +1720,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{227B468A-D31B-4B26-AB25-82ACAC0160B1}">
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{227B468A-D31B-4B26-AB25-82ACAC0160B1}">
       <text>
         <r>
           <rPr>
@@ -1802,7 +1744,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{6B04D491-22C5-4C9D-8E0F-C5484E44DCCD}">
+    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{6B04D491-22C5-4C9D-8E0F-C5484E44DCCD}">
       <text>
         <r>
           <rPr>
@@ -1826,7 +1768,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{FC9B2166-9A6E-4D98-AD30-E36CE6C3D758}">
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{FC9B2166-9A6E-4D98-AD30-E36CE6C3D758}">
       <text>
         <r>
           <rPr>
@@ -1898,7 +1840,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J4" authorId="0" shapeId="0" xr:uid="{D9359061-947C-4991-B1EC-3FEF9F5D7A82}">
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{D9359061-947C-4991-B1EC-3FEF9F5D7A82}">
       <text>
         <r>
           <rPr>
@@ -1970,7 +1912,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{B7E1B3AF-3A44-4383-BFA8-257E2C687078}">
+    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{B7E1B3AF-3A44-4383-BFA8-257E2C687078}">
       <text>
         <r>
           <rPr>
@@ -2105,7 +2047,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="132">
   <si>
     <t>monetary</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2207,10 +2149,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>#107c41</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>#094926</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2337,21 +2275,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>#107c42</t>
-  </si>
-  <si>
-    <t>#107c43</t>
-  </si>
-  <si>
-    <t>#107c44</t>
-  </si>
-  <si>
-    <t>#107c45</t>
-  </si>
-  <si>
-    <t>#107c46</t>
-  </si>
-  <si>
     <t>#c69872</t>
   </si>
   <si>
@@ -2494,10 +2417,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>interest_rate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>primary_carrier_out</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2621,6 +2540,25 @@
   </si>
   <si>
     <t>supply_for_pv</t>
+  </si>
+  <si>
+    <t>district_heating</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASHP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GSHP</t>
+  </si>
+  <si>
+    <t>GSHP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>water_tank</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2631,14 +2569,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2660,26 +2598,26 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -3084,26 +3022,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2603C43B-861B-457A-A24B-3EBFF53534AD}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
-    <col min="1" max="1" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.875" customWidth="1"/>
-    <col min="7" max="7" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.35546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.35546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.35546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15">
+    <row r="1" spans="1:7">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -3114,28 +3050,24 @@
         <v>23</v>
       </c>
       <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15">
+    <row r="2" spans="1:7">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8" t="s">
+      <c r="F2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" ht="15">
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -3143,94 +3075,76 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>100</v>
+        <v>16</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="I3" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4">
         <v>0.2505</v>
       </c>
       <c r="F4">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="G4">
-        <v>0.02</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5">
         <v>0.13250000000000001</v>
       </c>
       <c r="F5">
-        <v>0.05</v>
+        <v>0.23</v>
       </c>
       <c r="G5">
-        <v>0.23</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -3239,27 +3153,21 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="F6">
-        <v>0.05</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="G6">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -3268,27 +3176,21 @@
         <v>0.1</v>
       </c>
       <c r="F7">
-        <v>0.05</v>
+        <v>0.32400000000000001</v>
       </c>
       <c r="G7">
-        <v>0.32400000000000001</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -3297,25 +3199,17 @@
         <v>0.122</v>
       </c>
       <c r="F8">
-        <v>0.05</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="G8">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="3">
     <mergeCell ref="A1:D2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3325,35 +3219,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{561E90E2-20B4-48EB-B5A5-7E82D5B88F8D}">
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
-    <col min="1" max="1" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.35546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.875" customWidth="1"/>
-    <col min="7" max="7" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.875" customWidth="1"/>
-    <col min="11" max="11" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.125" customWidth="1"/>
-    <col min="13" max="13" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.35546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15">
+    <row r="1" spans="1:14">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -3365,21 +3255,17 @@
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="H1" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
-      <c r="K1" s="8" t="s">
-        <v>19</v>
-      </c>
+      <c r="K1" s="8"/>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-    </row>
-    <row r="2" spans="1:18" ht="15">
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -3388,22 +3274,18 @@
         <v>0</v>
       </c>
       <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="H2" s="8"/>
-      <c r="I2" s="8" t="s">
-        <v>18</v>
-      </c>
+      <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-    </row>
-    <row r="3" spans="1:18" ht="15">
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -3411,162 +3293,134 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>99</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>14</v>
+        <v>121</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>77</v>
+        <v>22</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="R3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E4">
         <v>3000</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="P4">
+      <c r="L4">
         <v>1</v>
       </c>
-      <c r="Q4">
+      <c r="M4">
         <v>10</v>
       </c>
-      <c r="R4">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E5">
         <v>1600</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="P5">
+      <c r="L5">
         <v>10</v>
       </c>
-      <c r="Q5">
+      <c r="M5">
         <v>100</v>
       </c>
-      <c r="R5">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E6">
         <v>1300</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="P6">
+      <c r="L6">
         <v>100</v>
       </c>
-      <c r="Q6">
+      <c r="M6">
         <v>200</v>
       </c>
-      <c r="R6">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E7">
         <v>1000</v>
       </c>
-      <c r="G7" s="7"/>
-      <c r="P7">
+      <c r="L7">
         <v>200</v>
       </c>
-      <c r="Q7">
+      <c r="M7">
         <v>2000</v>
       </c>
-      <c r="R7">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D8" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E8">
         <v>1576</v>
@@ -3574,46 +3428,40 @@
       <c r="F8">
         <v>1</v>
       </c>
-      <c r="H8">
-        <v>0.05</v>
-      </c>
-      <c r="I8">
+      <c r="G8">
         <v>290</v>
       </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8" t="s">
-        <v>108</v>
-      </c>
-      <c r="L8" t="b">
+      <c r="H8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I8" t="b">
         <v>1</v>
       </c>
-      <c r="M8" t="s">
-        <v>78</v>
+      <c r="J8" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8">
+        <v>1.2969999999999999</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
       </c>
       <c r="N8">
-        <v>1.2969999999999999</v>
-      </c>
-      <c r="P8">
-        <v>1</v>
-      </c>
-      <c r="R8">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9">
         <v>2047</v>
@@ -3621,41 +3469,34 @@
       <c r="F9">
         <v>1</v>
       </c>
-      <c r="H9">
-        <v>0.05</v>
-      </c>
-      <c r="I9">
+      <c r="G9">
         <v>296</v>
       </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9" t="s">
-        <v>107</v>
-      </c>
-      <c r="L9" t="b">
+      <c r="H9" t="s">
+        <v>100</v>
+      </c>
+      <c r="I9" t="b">
         <v>1</v>
       </c>
-      <c r="M9" t="s">
-        <v>78</v>
+      <c r="J9" t="s">
+        <v>72</v>
+      </c>
+      <c r="K9">
+        <v>1.41</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
       </c>
       <c r="N9">
-        <v>1.41</v>
-      </c>
-      <c r="P9">
-        <v>1</v>
-      </c>
-      <c r="R9">
         <v>23</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="K1:R2"/>
+  <mergeCells count="4">
+    <mergeCell ref="H1:N2"/>
     <mergeCell ref="A1:D2"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E1:G1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3665,32 +3506,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A246388-C9BA-4771-92A8-398DB13C28C5}">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
-    <col min="1" max="1" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.35546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.875" customWidth="1"/>
-    <col min="12" max="12" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.35546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.2109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15">
+    <row r="1" spans="1:13">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -3704,16 +3542,14 @@
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
+      <c r="J1" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="K1" s="8"/>
-      <c r="L1" s="8" t="s">
-        <v>19</v>
-      </c>
+      <c r="L1" s="8"/>
       <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-    </row>
-    <row r="2" spans="1:15" ht="15">
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -3724,17 +3560,15 @@
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8" t="s">
+      <c r="I2" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-    </row>
-    <row r="3" spans="1:15" ht="15">
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -3742,997 +3576,636 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>99</v>
+        <v>13</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>48</v>
+        <v>127</v>
       </c>
       <c r="F4">
         <v>371.80000000000013</v>
       </c>
       <c r="G4">
-        <v>0.05</v>
-      </c>
-      <c r="H4">
         <v>7322.9999999999964</v>
       </c>
-      <c r="I4">
-        <v>150</v>
-      </c>
-      <c r="J4">
-        <v>4.7709999999999999</v>
-      </c>
       <c r="K4">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="L4">
-        <v>0.95</v>
-      </c>
-      <c r="M4">
-        <v>15</v>
-      </c>
-      <c r="N4">
         <v>50</v>
       </c>
-      <c r="O4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>48</v>
+        <v>127</v>
       </c>
       <c r="F5">
         <v>180.88</v>
       </c>
       <c r="G5">
-        <v>0.05</v>
-      </c>
-      <c r="H5">
         <v>16869</v>
       </c>
-      <c r="I5">
-        <v>150</v>
-      </c>
-      <c r="J5">
-        <v>4.7709999999999999</v>
-      </c>
       <c r="K5">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="L5">
-        <v>0.95</v>
-      </c>
-      <c r="M5">
-        <v>50</v>
-      </c>
-      <c r="N5">
         <v>200</v>
       </c>
-      <c r="O5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>48</v>
+        <v>127</v>
       </c>
       <c r="F6">
         <v>117.4</v>
       </c>
       <c r="G6">
-        <v>0.05</v>
-      </c>
-      <c r="H6">
         <v>29571.7</v>
       </c>
-      <c r="I6">
-        <v>150</v>
-      </c>
-      <c r="J6">
-        <v>4.7709999999999999</v>
-      </c>
       <c r="K6">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="L6">
-        <v>0.95</v>
-      </c>
-      <c r="M6">
-        <v>200</v>
-      </c>
-      <c r="N6">
         <v>500</v>
       </c>
-      <c r="O6">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" t="s">
-        <v>48</v>
+        <v>127</v>
       </c>
       <c r="F7">
         <v>72.010000000000005</v>
       </c>
       <c r="G7">
-        <v>0.05</v>
-      </c>
-      <c r="H7">
         <v>52250</v>
       </c>
-      <c r="I7">
-        <v>150</v>
-      </c>
-      <c r="J7">
-        <v>4.7709999999999999</v>
-      </c>
       <c r="K7">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="L7">
-        <v>0.95</v>
-      </c>
-      <c r="M7">
-        <v>500</v>
-      </c>
-      <c r="N7">
         <v>2000</v>
       </c>
-      <c r="O7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8">
+        <v>4.58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E9" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9">
+        <v>7.64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10">
+        <v>2.89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E11" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11">
+        <v>4.13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="J12">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+      <c r="J13">
+        <v>2.96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" t="s">
         <v>32</v>
       </c>
-      <c r="E8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8">
-        <v>1814.5</v>
-      </c>
-      <c r="G8">
-        <v>0.05</v>
-      </c>
-      <c r="H8">
-        <v>12655</v>
-      </c>
-      <c r="I8">
-        <v>4.6399999999999997</v>
-      </c>
-      <c r="J8">
-        <v>45.9</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>4.58</v>
-      </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8">
-        <v>200</v>
-      </c>
-      <c r="O8">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" t="s">
-        <v>96</v>
-      </c>
-      <c r="D9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9">
-        <v>2544.9</v>
-      </c>
-      <c r="G9">
-        <v>0.05</v>
-      </c>
-      <c r="H9">
-        <v>37064</v>
-      </c>
-      <c r="I9">
-        <v>11.57</v>
-      </c>
-      <c r="J9">
-        <v>36.299999999999997</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>7.64</v>
-      </c>
-      <c r="M9">
-        <v>5</v>
-      </c>
-      <c r="N9">
-        <v>1000</v>
-      </c>
-      <c r="O9">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10">
-        <v>1814.5</v>
-      </c>
-      <c r="G10">
-        <v>0.05</v>
-      </c>
-      <c r="H10">
-        <v>12655</v>
-      </c>
-      <c r="I10">
-        <v>4.6399999999999997</v>
-      </c>
-      <c r="J10">
-        <v>45.9</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>2.89</v>
-      </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
-      <c r="N10">
-        <v>200</v>
-      </c>
-      <c r="O10">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" t="s">
-        <v>96</v>
-      </c>
-      <c r="D11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11">
-        <v>2544.9</v>
-      </c>
-      <c r="G11">
-        <v>0.05</v>
-      </c>
-      <c r="H11">
-        <v>37064</v>
-      </c>
-      <c r="I11">
-        <v>11.57</v>
-      </c>
-      <c r="J11">
-        <v>36.299999999999997</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>4.13</v>
-      </c>
-      <c r="M11">
-        <v>5</v>
-      </c>
-      <c r="N11">
-        <v>1000</v>
-      </c>
-      <c r="O11">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" t="s">
-        <v>96</v>
-      </c>
-      <c r="D12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12">
-        <v>1814.5</v>
-      </c>
-      <c r="G12">
-        <v>0.05</v>
-      </c>
-      <c r="H12">
-        <v>12655</v>
-      </c>
-      <c r="I12">
-        <v>4.6399999999999997</v>
-      </c>
-      <c r="J12">
-        <v>45.9</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
-      <c r="N12">
-        <v>200</v>
-      </c>
-      <c r="O12">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" t="s">
-        <v>84</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" t="s">
-        <v>96</v>
-      </c>
-      <c r="D13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13">
-        <v>2544.9</v>
-      </c>
-      <c r="G13">
-        <v>0.05</v>
-      </c>
-      <c r="H13">
-        <v>37064</v>
-      </c>
-      <c r="I13">
-        <v>11.57</v>
-      </c>
-      <c r="J13">
-        <v>36.299999999999997</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>2.96</v>
-      </c>
-      <c r="M13">
-        <v>5</v>
-      </c>
-      <c r="N13">
-        <v>1000</v>
-      </c>
-      <c r="O13">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" t="s">
-        <v>96</v>
-      </c>
-      <c r="D14" t="s">
-        <v>33</v>
-      </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F14">
         <v>300</v>
       </c>
       <c r="G14">
-        <v>0.05</v>
+        <v>17200</v>
       </c>
       <c r="H14">
-        <v>17200</v>
+        <v>6.3</v>
       </c>
       <c r="I14">
-        <v>6.3</v>
+        <v>37.685000000000002</v>
       </c>
       <c r="J14">
-        <v>37.685000000000002</v>
+        <v>0.91</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14">
-        <v>0.91</v>
+        <v>20</v>
       </c>
       <c r="M14">
-        <v>1</v>
-      </c>
-      <c r="N14">
         <v>20</v>
       </c>
-      <c r="O14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F15">
         <v>880</v>
       </c>
       <c r="G15">
-        <v>0.05</v>
+        <v>25100</v>
       </c>
       <c r="H15">
-        <v>25100</v>
+        <v>6.3</v>
       </c>
       <c r="I15">
-        <v>6.3</v>
+        <v>77.900000000000006</v>
       </c>
       <c r="J15">
-        <v>77.900000000000006</v>
+        <v>0.89</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15">
-        <v>0.89</v>
+        <v>20</v>
       </c>
       <c r="M15">
-        <v>1</v>
-      </c>
-      <c r="N15">
         <v>20</v>
       </c>
-      <c r="O15">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F16">
         <v>486.7</v>
       </c>
       <c r="G16">
-        <v>0.05</v>
+        <v>20466.7</v>
       </c>
       <c r="H16">
-        <v>20466.7</v>
+        <v>3.5</v>
       </c>
       <c r="I16">
-        <v>3.5</v>
+        <v>44.555</v>
       </c>
       <c r="J16">
-        <v>44.555</v>
+        <v>0.92</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16">
-        <v>0.92</v>
+        <v>20</v>
       </c>
       <c r="M16">
-        <v>1</v>
-      </c>
-      <c r="N16">
         <v>20</v>
       </c>
-      <c r="O16">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F17">
         <v>176.7</v>
       </c>
       <c r="G17">
-        <v>0.05</v>
+        <v>19666.7</v>
       </c>
       <c r="H17">
-        <v>19666.7</v>
+        <v>6.3</v>
       </c>
       <c r="I17">
-        <v>6.3</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="J17">
-        <v>18.100000000000001</v>
+        <v>0.91</v>
       </c>
       <c r="K17">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L17">
-        <v>0.91</v>
+        <v>200</v>
       </c>
       <c r="M17">
-        <v>20</v>
-      </c>
-      <c r="N17">
-        <v>200</v>
-      </c>
-      <c r="O17">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D18" t="s">
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F18">
         <v>414.99999999999989</v>
       </c>
       <c r="G18">
-        <v>0.05</v>
+        <v>34400.000000000015</v>
       </c>
       <c r="H18">
-        <v>34400.000000000015</v>
+        <v>6.3</v>
       </c>
       <c r="I18">
-        <v>6.3</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="J18">
-        <v>19.399999999999999</v>
+        <v>0.89</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L18">
-        <v>0.89</v>
+        <v>200</v>
       </c>
       <c r="M18">
         <v>20</v>
       </c>
-      <c r="N18">
-        <v>200</v>
-      </c>
-      <c r="O18">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15">
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F19">
         <v>189.4</v>
       </c>
       <c r="G19">
-        <v>0.05</v>
+        <v>26411.1</v>
       </c>
       <c r="H19">
-        <v>26411.1</v>
+        <v>3.5</v>
       </c>
       <c r="I19">
-        <v>3.5</v>
+        <v>25.07</v>
       </c>
       <c r="J19">
-        <v>25.07</v>
+        <v>0.92</v>
       </c>
       <c r="K19">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L19">
-        <v>0.92</v>
+        <v>200</v>
       </c>
       <c r="M19">
         <v>20</v>
       </c>
-      <c r="N19">
-        <v>200</v>
-      </c>
-      <c r="O19">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15">
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F20">
         <v>155.30000000000001</v>
       </c>
       <c r="G20">
-        <v>0.05</v>
+        <v>23933.3</v>
       </c>
       <c r="H20">
-        <v>23933.3</v>
+        <v>6.3</v>
       </c>
       <c r="I20">
-        <v>6.3</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="J20">
-        <v>18.100000000000001</v>
+        <v>0.91</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="L20">
-        <v>0.91</v>
+        <v>500</v>
       </c>
       <c r="M20">
-        <v>200</v>
-      </c>
-      <c r="N20">
-        <v>500</v>
-      </c>
-      <c r="O20">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D21" t="s">
         <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F21">
         <v>278.00000000000006</v>
       </c>
       <c r="G21">
-        <v>0.05</v>
+        <v>61799.999999999985</v>
       </c>
       <c r="H21">
-        <v>61799.999999999985</v>
+        <v>6.3</v>
       </c>
       <c r="I21">
-        <v>6.3</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="J21">
-        <v>19.399999999999999</v>
+        <v>0.89</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="L21">
-        <v>0.89</v>
+        <v>500</v>
       </c>
       <c r="M21">
-        <v>200</v>
-      </c>
-      <c r="N21">
-        <v>500</v>
-      </c>
-      <c r="O21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F22">
         <v>211.7</v>
       </c>
       <c r="G22">
-        <v>0.05</v>
+        <v>21966.7</v>
       </c>
       <c r="H22">
-        <v>21966.7</v>
+        <v>3.5</v>
       </c>
       <c r="I22">
-        <v>3.5</v>
+        <v>19.510000000000002</v>
       </c>
       <c r="J22">
-        <v>19.510000000000002</v>
+        <v>0.92</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="L22">
-        <v>0.92</v>
+        <v>500</v>
       </c>
       <c r="M22">
-        <v>200</v>
-      </c>
-      <c r="N22">
-        <v>500</v>
-      </c>
-      <c r="O22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C23" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E23" t="s">
-        <v>75</v>
-      </c>
-      <c r="G23">
-        <v>0.05</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
+        <v>69</v>
+      </c>
+      <c r="J23">
         <v>1</v>
       </c>
-      <c r="O23">
+      <c r="M23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D24" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E24" t="s">
-        <v>51</v>
-      </c>
-      <c r="G24">
-        <v>0.05</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
+        <v>50</v>
+      </c>
+      <c r="J24">
         <v>1</v>
       </c>
-      <c r="O24">
+      <c r="M24">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A1:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="L1:O2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="J1:M2"/>
+    <mergeCell ref="F1:I1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4745,37 +4218,37 @@
   <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
-    <col min="1" max="1" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.35546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.2109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.2109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.625" customWidth="1"/>
-    <col min="17" max="17" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.25" customWidth="1"/>
-    <col min="22" max="22" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.640625" customWidth="1"/>
+    <col min="17" max="17" width="10.2109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.2109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.2109375" customWidth="1"/>
+    <col min="22" max="22" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15">
+    <row r="1" spans="1:24">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -4807,7 +4280,7 @@
       <c r="W1" s="8"/>
       <c r="X1" s="8"/>
     </row>
-    <row r="2" spans="1:24" ht="15">
+    <row r="2" spans="1:24">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -4837,7 +4310,7 @@
       <c r="W2" s="8"/>
       <c r="X2" s="8"/>
     </row>
-    <row r="3" spans="1:24" ht="15">
+    <row r="3" spans="1:24">
       <c r="A3" s="8" t="s">
         <v>24</v>
       </c>
@@ -4845,34 +4318,34 @@
         <v>7</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>14</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="M3" s="8" t="s">
         <v>13</v>
@@ -4884,18 +4357,18 @@
         <v>14</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Q3" s="8" t="s">
         <v>20</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="S3" s="9"/>
       <c r="T3" s="9"/>
       <c r="U3" s="9" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="V3" s="8" t="s">
         <v>21</v>
@@ -4907,7 +4380,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="15">
+    <row r="4" spans="1:24">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -4926,18 +4399,18 @@
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
       <c r="R4" s="9" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="S4" s="9"/>
       <c r="T4" s="6" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="U4" s="9"/>
       <c r="V4" s="8"/>
       <c r="W4" s="8"/>
       <c r="X4" s="8"/>
     </row>
-    <row r="5" spans="1:24" ht="15">
+    <row r="5" spans="1:24">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -4956,37 +4429,37 @@
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U5" s="9"/>
       <c r="V5" s="8"/>
       <c r="W5" s="8"/>
       <c r="X5" s="8"/>
     </row>
-    <row r="6" spans="1:24" ht="14.25">
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="H6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="J6">
         <v>1108.2</v>
@@ -5018,7 +4491,7 @@
         <v>0.64</v>
       </c>
       <c r="U6" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V6">
         <v>10</v>
@@ -5032,6 +4505,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="Q3:Q5"/>
+    <mergeCell ref="W3:W5"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="U3:U5"/>
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="J1:P1"/>
     <mergeCell ref="D3:D5"/>
@@ -5048,18 +4533,6 @@
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="X3:X5"/>
     <mergeCell ref="A1:I2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="Q3:Q5"/>
-    <mergeCell ref="W3:W5"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="I3:I5"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="U3:U5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5069,32 +4542,30 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED8072C-161B-4E9B-9246-F2F0563C6573}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.5" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="16.5" defaultRowHeight="14.15"/>
   <cols>
-    <col min="1" max="1" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.78515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.35546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.375" customWidth="1"/>
-    <col min="10" max="10" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.0703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.0703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.0703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15">
+    <row r="1" spans="1:13">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -5106,18 +4577,16 @@
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="H1" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="I1" s="8"/>
-      <c r="J1" s="8" t="s">
-        <v>19</v>
-      </c>
+      <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-    </row>
-    <row r="2" spans="1:15" ht="15">
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -5126,19 +4595,17 @@
         <v>0</v>
       </c>
       <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8" t="s">
+      <c r="G2" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="H2" s="8"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-    </row>
-    <row r="3" spans="1:15" ht="15">
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -5146,57 +4613,51 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>72</v>
+        <v>20</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="O3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="27">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4">
         <v>367</v>
@@ -5205,172 +4666,93 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="G4">
-        <v>0.05</v>
+        <v>241.5</v>
       </c>
       <c r="H4">
-        <v>241.5</v>
+        <v>0.91</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="J4">
-        <v>0.91</v>
+        <v>0.25</v>
       </c>
       <c r="K4">
-        <v>1000</v>
+        <v>1E-3</v>
       </c>
       <c r="L4">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="M4">
-        <v>1E-3</v>
-      </c>
-      <c r="N4">
-        <v>0.5</v>
-      </c>
-      <c r="O4">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="27">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5">
+        <v>0.96</v>
+      </c>
+      <c r="K5">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="H6">
+        <v>0.95</v>
+      </c>
+      <c r="K6">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5">
-        <v>13</v>
-      </c>
-      <c r="F5">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="G5">
-        <v>0.05</v>
-      </c>
-      <c r="H5">
-        <v>7</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0.96</v>
-      </c>
-      <c r="K5">
-        <v>1000</v>
-      </c>
-      <c r="M5">
-        <v>0.01</v>
-      </c>
-      <c r="N5">
-        <v>0.5</v>
-      </c>
-      <c r="O5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="27">
-      <c r="A6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E6">
-        <v>13</v>
-      </c>
-      <c r="F6">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="G6">
-        <v>0.05</v>
-      </c>
-      <c r="H6">
-        <v>7</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0.95</v>
-      </c>
-      <c r="K6">
-        <v>1000</v>
-      </c>
-      <c r="M6">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="N6">
-        <v>0.5</v>
-      </c>
-      <c r="O6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="27">
-      <c r="A7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7">
-        <v>13</v>
-      </c>
-      <c r="F7">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="G7">
-        <v>0.05</v>
+        <v>47</v>
       </c>
       <c r="H7">
-        <v>7</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
         <v>0.94</v>
       </c>
       <c r="K7">
-        <v>1000</v>
-      </c>
-      <c r="M7">
         <v>0.02</v>
       </c>
-      <c r="N7">
-        <v>0.5</v>
-      </c>
-      <c r="O7">
-        <v>23</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A1:D2"/>
-    <mergeCell ref="J1:O2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="H1:M2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E1:G1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5386,13 +4768,13 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
-    <col min="1" max="1" width="23.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.35546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.2109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -5413,7 +4795,7 @@
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" ht="15">
+    <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -5421,115 +4803,115 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" t="s">
         <v>109</v>
       </c>
-      <c r="B4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C4" t="s">
-        <v>116</v>
-      </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C5" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B6" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C6" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E6" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C7" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" t="s">
         <v>110</v>
       </c>
-      <c r="B8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C8" t="s">
-        <v>116</v>
-      </c>
-      <c r="D8" t="s">
-        <v>117</v>
-      </c>
       <c r="E8" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>